<commit_message>
added repos for courses
</commit_message>
<xml_diff>
--- a/salesboost-adminpanel/Excel/Data.xlsx
+++ b/salesboost-adminpanel/Excel/Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\workspace-spring-tool-suite-4-4.7.0.RELEASE\salesboost-adminpanel\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F660899D-4EFA-4F10-A0EB-FC22E507D53C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598353FA-235D-44F8-9535-1F84F6AF4347}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{0E4BCD85-B79C-44E4-BF30-FA11BE829E64}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="124">
   <si>
     <t>balu.kr@experionglobal.com</t>
   </si>
@@ -93,13 +93,325 @@
   </si>
   <si>
     <t>Exp Ayan</t>
+  </si>
+  <si>
+    <t>login password</t>
+  </si>
+  <si>
+    <t>manage password mail ---&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">login email </t>
+  </si>
+  <si>
+    <t>selection tab- show all(s) super(ss) admin(a) guest(g)</t>
+  </si>
+  <si>
+    <t>name of user to search</t>
+  </si>
+  <si>
+    <t>administrators</t>
+  </si>
+  <si>
+    <t>administrator mail id</t>
+  </si>
+  <si>
+    <t>admin first name</t>
+  </si>
+  <si>
+    <t>admin last name</t>
+  </si>
+  <si>
+    <t>level -guest(g) super(S) admin(a)</t>
+  </si>
+  <si>
+    <t>add user</t>
+  </si>
+  <si>
+    <t>edit user</t>
+  </si>
+  <si>
+    <t>account holders</t>
+  </si>
+  <si>
+    <t>selection tab- show all(s) basic(b) premium(p)</t>
+  </si>
+  <si>
+    <t>account name</t>
+  </si>
+  <si>
+    <t>level basic(b) premium(p)</t>
+  </si>
+  <si>
+    <t>type indiv(i) org(0)</t>
+  </si>
+  <si>
+    <t>owner first name</t>
+  </si>
+  <si>
+    <t>last name</t>
+  </si>
+  <si>
+    <t>owner email</t>
+  </si>
+  <si>
+    <t>add account</t>
+  </si>
+  <si>
+    <t>edit account</t>
+  </si>
+  <si>
+    <t>add whitelabel account</t>
+  </si>
+  <si>
+    <t>display name</t>
+  </si>
+  <si>
+    <t>host name</t>
+  </si>
+  <si>
+    <t>pr. Brand color</t>
+  </si>
+  <si>
+    <t>sec. color</t>
+  </si>
+  <si>
+    <t>accent color</t>
+  </si>
+  <si>
+    <t>head color</t>
+  </si>
+  <si>
+    <t>score color</t>
+  </si>
+  <si>
+    <t>track head color</t>
+  </si>
+  <si>
+    <t>track score color</t>
+  </si>
+  <si>
+    <t>private test</t>
+  </si>
+  <si>
+    <t>private tests</t>
+  </si>
+  <si>
+    <t>edit whitelabel account</t>
+  </si>
+  <si>
+    <t>private test1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">role management </t>
+  </si>
+  <si>
+    <t>selection- all(a) active(aa) inactive(i)</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>add role- role management</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>test role</t>
+  </si>
+  <si>
+    <t>test description</t>
+  </si>
+  <si>
+    <t>role list</t>
+  </si>
+  <si>
+    <t>role test</t>
+  </si>
+  <si>
+    <t>test description for aut.</t>
+  </si>
+  <si>
+    <t>EDIT role- role management</t>
+  </si>
+  <si>
+    <t>System announcements</t>
+  </si>
+  <si>
+    <t>role to be searched</t>
+  </si>
+  <si>
+    <t>announcement to search</t>
+  </si>
+  <si>
+    <t>selection- show all(s) active(aa) inactive(i)</t>
+  </si>
+  <si>
+    <t>add system announcements</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>sub title</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>seo title</t>
+  </si>
+  <si>
+    <t>seo decription</t>
+  </si>
+  <si>
+    <t>seo keyword</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>test announcement</t>
+  </si>
+  <si>
+    <t>test acc</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>test description for aut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test </t>
+  </si>
+  <si>
+    <t>aaaa</t>
+  </si>
+  <si>
+    <t>test content</t>
+  </si>
+  <si>
+    <t>edit system announcements</t>
+  </si>
+  <si>
+    <t>tags</t>
+  </si>
+  <si>
+    <t>posts</t>
+  </si>
+  <si>
+    <t>courses</t>
+  </si>
+  <si>
+    <t>test accts</t>
+  </si>
+  <si>
+    <t>abc.com</t>
+  </si>
+  <si>
+    <t>trial test course</t>
+  </si>
+  <si>
+    <t>tip to search</t>
+  </si>
+  <si>
+    <t>Quick sales tips</t>
+  </si>
+  <si>
+    <t>test tip</t>
+  </si>
+  <si>
+    <t>testtip</t>
+  </si>
+  <si>
+    <t>desc</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>ttc</t>
+  </si>
+  <si>
+    <t>test tips</t>
+  </si>
+  <si>
+    <t>tes tip</t>
+  </si>
+  <si>
+    <t>Leadership tips</t>
+  </si>
+  <si>
+    <t>add leadership tips</t>
+  </si>
+  <si>
+    <t>tip#</t>
+  </si>
+  <si>
+    <t>edit leadership tips</t>
+  </si>
+  <si>
+    <t>leadership tools</t>
+  </si>
+  <si>
+    <t>Add Leadership tools</t>
+  </si>
+  <si>
+    <t>short name</t>
+  </si>
+  <si>
+    <t>Edit leadership tools</t>
+  </si>
+  <si>
+    <t>Duplicate Leadership tools</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>Edit private leadership tools</t>
+  </si>
+  <si>
+    <t>Add private Leadership tools</t>
+  </si>
+  <si>
+    <t>Tracks</t>
+  </si>
+  <si>
+    <t>track to search</t>
+  </si>
+  <si>
+    <t>Add Track</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Slug</t>
+  </si>
+  <si>
+    <t>Desccription</t>
+  </si>
+  <si>
+    <t>Edit Track</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,13 +427,56 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -137,9 +492,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -455,120 +817,880 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{455EF352-F706-4455-ADF1-85E3A647B83A}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:P60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.5703125" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.85546875" customWidth="1"/>
+    <col min="1" max="1" width="50.85546875" customWidth="1"/>
+    <col min="2" max="2" width="48" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" customWidth="1"/>
+    <col min="4" max="4" width="35" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
     <col min="6" max="6" width="34.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="13" max="13" width="16" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C9" t="s">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B13" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C13" t="s">
         <v>9</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D13" t="s">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E13" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B15" t="s">
         <v>11</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C15" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" t="s">
+        <v>84</v>
+      </c>
+      <c r="F29" t="s">
+        <v>85</v>
+      </c>
+      <c r="G29" t="s">
+        <v>86</v>
+      </c>
+      <c r="H29" t="s">
+        <v>87</v>
+      </c>
+      <c r="I29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" t="s">
+        <v>94</v>
+      </c>
+      <c r="E31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F31" t="s">
+        <v>85</v>
+      </c>
+      <c r="G31" t="s">
+        <v>86</v>
+      </c>
+      <c r="H31" t="s">
+        <v>87</v>
+      </c>
+      <c r="I31" t="s">
+        <v>86</v>
+      </c>
+      <c r="J31" t="s">
+        <v>91</v>
+      </c>
+      <c r="K31" t="s">
+        <v>95</v>
+      </c>
+      <c r="L31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>98</v>
+      </c>
+      <c r="C35" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" t="s">
+        <v>84</v>
+      </c>
+      <c r="E35" t="s">
+        <v>100</v>
+      </c>
+      <c r="F35" t="s">
+        <v>101</v>
+      </c>
+      <c r="G35" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" t="s">
+        <v>104</v>
+      </c>
+      <c r="F37" t="s">
+        <v>101</v>
+      </c>
+      <c r="G37" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{D467F256-CF0A-4C81-803A-7096B63133F6}"/>
-    <hyperlink ref="A4" r:id="rId2" xr:uid="{2F5C6525-635C-4C7B-ACED-EDC4D4E45F3A}"/>
-    <hyperlink ref="A5" r:id="rId3" xr:uid="{B5351774-2290-4A1C-B0B5-7EC85B45A097}"/>
-    <hyperlink ref="F7" r:id="rId4" xr:uid="{411F89DF-4CDF-4F5E-A3B5-94C29B85EB49}"/>
-    <hyperlink ref="D8" r:id="rId5" xr:uid="{93626398-8389-47C9-926F-462B19FF1DB7}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{D467F256-CF0A-4C81-803A-7096B63133F6}"/>
+    <hyperlink ref="A7" r:id="rId2" xr:uid="{2F5C6525-635C-4C7B-ACED-EDC4D4E45F3A}"/>
+    <hyperlink ref="A9" r:id="rId3" xr:uid="{B5351774-2290-4A1C-B0B5-7EC85B45A097}"/>
+    <hyperlink ref="F13" r:id="rId4" xr:uid="{411F89DF-4CDF-4F5E-A3B5-94C29B85EB49}"/>
+    <hyperlink ref="D15" r:id="rId5" xr:uid="{93626398-8389-47C9-926F-462B19FF1DB7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
push with code changes in test script
</commit_message>
<xml_diff>
--- a/salesboost-adminpanel/Excel/Data.xlsx
+++ b/salesboost-adminpanel/Excel/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\workspace-spring-tool-suite-4-4.7.0.RELEASE\salesboost-adminpanel\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598353FA-235D-44F8-9535-1F84F6AF4347}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53BA7DB-FB4F-4ED1-9DFD-76E408055CD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{0E4BCD85-B79C-44E4-BF30-FA11BE829E64}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="129">
   <si>
     <t>balu.kr@experionglobal.com</t>
   </si>
@@ -405,6 +405,21 @@
   </si>
   <si>
     <t>Edit Track</t>
+  </si>
+  <si>
+    <t>test track</t>
+  </si>
+  <si>
+    <t>this is  a  test track for aut.</t>
+  </si>
+  <si>
+    <t>track test</t>
+  </si>
+  <si>
+    <t>add sales tips</t>
+  </si>
+  <si>
+    <t>edit sales tips</t>
   </si>
 </sst>
 </file>
@@ -817,10 +832,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{455EF352-F706-4455-ADF1-85E3A647B83A}">
-  <dimension ref="A1:P60"/>
+  <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1390,7 +1405,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>72</v>
+        <v>127</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>73</v>
@@ -1433,7 +1448,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>89</v>
+        <v>128</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>73</v>
@@ -1648,6 +1663,14 @@
         <v>118</v>
       </c>
     </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" t="s">
+        <v>84</v>
+      </c>
+    </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
         <v>119</v>
@@ -1662,6 +1685,17 @@
         <v>122</v>
       </c>
     </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>124</v>
+      </c>
+      <c r="C59" t="s">
+        <v>84</v>
+      </c>
+      <c r="D59" t="s">
+        <v>125</v>
+      </c>
+    </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
         <v>123</v>
@@ -1680,6 +1714,23 @@
       </c>
       <c r="F60" s="2" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>84</v>
+      </c>
+      <c r="C61" t="s">
+        <v>126</v>
+      </c>
+      <c r="D61" t="s">
+        <v>125</v>
+      </c>
+      <c r="E61" t="s">
+        <v>102</v>
+      </c>
+      <c r="F61" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
push with modified script for role
</commit_message>
<xml_diff>
--- a/salesboost-adminpanel/Excel/Data.xlsx
+++ b/salesboost-adminpanel/Excel/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\workspace-spring-tool-suite-4-4.7.0.RELEASE\salesboost-adminpanel\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53BA7DB-FB4F-4ED1-9DFD-76E408055CD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF716539-EA3E-4608-A6FA-D781D60A9627}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{0E4BCD85-B79C-44E4-BF30-FA11BE829E64}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="136">
   <si>
     <t>balu.kr@experionglobal.com</t>
   </si>
@@ -420,6 +420,27 @@
   </si>
   <si>
     <t>edit sales tips</t>
+  </si>
+  <si>
+    <t>test tool</t>
+  </si>
+  <si>
+    <t>tts</t>
+  </si>
+  <si>
+    <t>tool test</t>
+  </si>
+  <si>
+    <t>ttt</t>
+  </si>
+  <si>
+    <t>duplicate test tool</t>
+  </si>
+  <si>
+    <t>dtt</t>
+  </si>
+  <si>
+    <t>Presenting Creative Solutions Tool Kit</t>
   </si>
 </sst>
 </file>
@@ -834,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{455EF352-F706-4455-ADF1-85E3A647B83A}">
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1575,6 +1596,9 @@
       <c r="B45" t="s">
         <v>58</v>
       </c>
+      <c r="C45" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
@@ -1590,6 +1614,17 @@
         <v>61</v>
       </c>
     </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>129</v>
+      </c>
+      <c r="C47" t="s">
+        <v>130</v>
+      </c>
+      <c r="D47" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>112</v>
@@ -1604,6 +1639,17 @@
         <v>61</v>
       </c>
     </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>131</v>
+      </c>
+      <c r="C49" t="s">
+        <v>132</v>
+      </c>
+      <c r="D49" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>113</v>
@@ -1616,6 +1662,17 @@
       </c>
       <c r="D50" s="2" t="s">
         <v>114</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>133</v>
+      </c>
+      <c r="C51" t="s">
+        <v>134</v>
+      </c>
+      <c r="D51" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
push with corrected scripts for sales
</commit_message>
<xml_diff>
--- a/salesboost-adminpanel/Excel/Data.xlsx
+++ b/salesboost-adminpanel/Excel/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\workspace-spring-tool-suite-4-4.7.0.RELEASE\salesboost-adminpanel\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF716539-EA3E-4608-A6FA-D781D60A9627}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79ABB0F7-A58D-4F63-8213-FCFDEE4E0A5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{0E4BCD85-B79C-44E4-BF30-FA11BE829E64}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="144">
   <si>
     <t>balu.kr@experionglobal.com</t>
   </si>
@@ -441,6 +441,30 @@
   </si>
   <si>
     <t>Presenting Creative Solutions Tool Kit</t>
+  </si>
+  <si>
+    <t>test slug</t>
+  </si>
+  <si>
+    <t>tip test</t>
+  </si>
+  <si>
+    <t>tc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> test c</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ttc </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> abc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> test</t>
   </si>
 </sst>
 </file>
@@ -855,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{455EF352-F706-4455-ADF1-85E3A647B83A}">
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="C27" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,7 +891,7 @@
     <col min="4" max="4" width="35" customWidth="1"/>
     <col min="5" max="5" width="13.140625" customWidth="1"/>
     <col min="6" max="6" width="34.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" customWidth="1"/>
     <col min="9" max="9" width="17.5703125" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
@@ -1423,6 +1447,9 @@
       <c r="B33" t="s">
         <v>10</v>
       </c>
+      <c r="C33" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
@@ -1464,7 +1491,7 @@
         <v>101</v>
       </c>
       <c r="G35" t="s">
-        <v>88</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -1497,14 +1524,23 @@
       <c r="B37" t="s">
         <v>103</v>
       </c>
+      <c r="C37" t="s">
+        <v>99</v>
+      </c>
       <c r="D37" t="s">
         <v>104</v>
       </c>
+      <c r="E37" t="s">
+        <v>100</v>
+      </c>
       <c r="F37" t="s">
         <v>101</v>
       </c>
       <c r="G37" t="s">
-        <v>102</v>
+        <v>141</v>
+      </c>
+      <c r="H37" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -1522,6 +1558,9 @@
       <c r="B39" t="s">
         <v>10</v>
       </c>
+      <c r="C39" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
@@ -1549,6 +1588,29 @@
         <v>80</v>
       </c>
     </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41">
+        <v>12</v>
+      </c>
+      <c r="D41" t="s">
+        <v>136</v>
+      </c>
+      <c r="E41" t="s">
+        <v>84</v>
+      </c>
+      <c r="F41" t="s">
+        <v>100</v>
+      </c>
+      <c r="G41" t="s">
+        <v>102</v>
+      </c>
+      <c r="H41" t="s">
+        <v>139</v>
+      </c>
+    </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>108</v>
@@ -1579,6 +1641,35 @@
       </c>
       <c r="J42" s="2" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>137</v>
+      </c>
+      <c r="C43">
+        <v>12</v>
+      </c>
+      <c r="D43" t="s">
+        <v>136</v>
+      </c>
+      <c r="E43" t="s">
+        <v>98</v>
+      </c>
+      <c r="F43" t="s">
+        <v>100</v>
+      </c>
+      <c r="G43" t="s">
+        <v>138</v>
+      </c>
+      <c r="H43" t="s">
+        <v>102</v>
+      </c>
+      <c r="I43" t="s">
+        <v>143</v>
+      </c>
+      <c r="J43" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
modified and corrected script for role management
</commit_message>
<xml_diff>
--- a/salesboost-adminpanel/Excel/Data.xlsx
+++ b/salesboost-adminpanel/Excel/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\workspace-spring-tool-suite-4-4.7.0.RELEASE\salesboost-adminpanel\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79ABB0F7-A58D-4F63-8213-FCFDEE4E0A5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA90087-081B-4822-831F-FAA72EC98530}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{0E4BCD85-B79C-44E4-BF30-FA11BE829E64}"/>
   </bookViews>
@@ -233,9 +233,6 @@
     <t>role test</t>
   </si>
   <si>
-    <t>test description for aut.</t>
-  </si>
-  <si>
     <t>EDIT role- role management</t>
   </si>
   <si>
@@ -465,6 +462,9 @@
   </si>
   <si>
     <t xml:space="preserve"> test</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> test description for aut.</t>
   </si>
 </sst>
 </file>
@@ -879,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{455EF352-F706-4455-ADF1-85E3A647B83A}">
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C27" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,7 +1230,7 @@
         <v>57</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -1262,7 +1262,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>60</v>
@@ -1279,7 +1279,7 @@
         <v>65</v>
       </c>
       <c r="C25" t="s">
-        <v>66</v>
+        <v>143</v>
       </c>
       <c r="D25" t="s">
         <v>7</v>
@@ -1287,13 +1287,13 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -1301,146 +1301,146 @@
         <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="G28" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="H28" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="I28" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" t="s">
         <v>81</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>82</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>83</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>84</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>85</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>86</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>87</v>
-      </c>
-      <c r="I29" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I30" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="H30" s="2" t="s">
+      <c r="J30" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L30" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" t="s">
         <v>93</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
+        <v>83</v>
+      </c>
+      <c r="F31" t="s">
+        <v>84</v>
+      </c>
+      <c r="G31" t="s">
+        <v>85</v>
+      </c>
+      <c r="H31" t="s">
+        <v>86</v>
+      </c>
+      <c r="I31" t="s">
+        <v>85</v>
+      </c>
+      <c r="J31" t="s">
+        <v>90</v>
+      </c>
+      <c r="K31" t="s">
         <v>94</v>
       </c>
-      <c r="E31" t="s">
-        <v>84</v>
-      </c>
-      <c r="F31" t="s">
-        <v>85</v>
-      </c>
-      <c r="G31" t="s">
-        <v>86</v>
-      </c>
-      <c r="H31" t="s">
+      <c r="L31" t="s">
         <v>87</v>
-      </c>
-      <c r="I31" t="s">
-        <v>86</v>
-      </c>
-      <c r="J31" t="s">
-        <v>91</v>
-      </c>
-      <c r="K31" t="s">
-        <v>95</v>
-      </c>
-      <c r="L31" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -1448,110 +1448,110 @@
         <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="G34" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" t="s">
         <v>98</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
+        <v>83</v>
+      </c>
+      <c r="E35" t="s">
         <v>99</v>
       </c>
-      <c r="D35" t="s">
-        <v>84</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>100</v>
       </c>
-      <c r="F35" t="s">
-        <v>101</v>
-      </c>
       <c r="G35" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="G36" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" t="s">
         <v>103</v>
       </c>
-      <c r="C37" t="s">
+      <c r="E37" t="s">
         <v>99</v>
       </c>
-      <c r="D37" t="s">
-        <v>104</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>100</v>
       </c>
-      <c r="F37" t="s">
-        <v>101</v>
-      </c>
       <c r="G37" t="s">
+        <v>140</v>
+      </c>
+      <c r="H37" t="s">
         <v>141</v>
-      </c>
-      <c r="H37" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -1559,128 +1559,128 @@
         <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="D40" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="F40" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="G40" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G40" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="H40" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C41">
         <v>12</v>
       </c>
       <c r="D41" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F41" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H41" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D42" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="F42" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="G42" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G42" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="H42" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I42" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="I42" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="J42" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C43">
         <v>12</v>
       </c>
       <c r="D43" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E43" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G43" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I43" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J43" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -1688,18 +1688,18 @@
         <v>58</v>
       </c>
       <c r="C45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>61</v>
@@ -1707,10 +1707,10 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
+        <v>128</v>
+      </c>
+      <c r="C47" t="s">
         <v>129</v>
-      </c>
-      <c r="C47" t="s">
-        <v>130</v>
       </c>
       <c r="D47" t="s">
         <v>61</v>
@@ -1718,13 +1718,13 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>61</v>
@@ -1732,10 +1732,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
+        <v>130</v>
+      </c>
+      <c r="C49" t="s">
         <v>131</v>
-      </c>
-      <c r="C49" t="s">
-        <v>132</v>
       </c>
       <c r="D49" t="s">
         <v>61</v>
@@ -1743,41 +1743,41 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
+        <v>132</v>
+      </c>
+      <c r="C51" t="s">
         <v>133</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>134</v>
-      </c>
-      <c r="D51" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>61</v>
@@ -1785,16 +1785,16 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>61</v>
@@ -1802,13 +1802,13 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -1816,69 +1816,69 @@
         <v>10</v>
       </c>
       <c r="C57" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="D58" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
+        <v>123</v>
+      </c>
+      <c r="C59" t="s">
+        <v>83</v>
+      </c>
+      <c r="D59" t="s">
         <v>124</v>
-      </c>
-      <c r="C59" t="s">
-        <v>84</v>
-      </c>
-      <c r="D59" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B60" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>122</v>
-      </c>
       <c r="E60" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C61" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D61" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E61" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F61" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all changes in test script
</commit_message>
<xml_diff>
--- a/salesboost-adminpanel/Excel/Data.xlsx
+++ b/salesboost-adminpanel/Excel/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\workspace-spring-tool-suite-4-4.7.0.RELEASE\salesboost-adminpanel\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA90087-081B-4822-831F-FAA72EC98530}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A342D60F-295E-445C-A5C4-B7E48A1E60DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{0E4BCD85-B79C-44E4-BF30-FA11BE829E64}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="157">
   <si>
     <t>balu.kr@experionglobal.com</t>
   </si>
@@ -465,6 +465,45 @@
   </si>
   <si>
     <t xml:space="preserve"> test description for aut.</t>
+  </si>
+  <si>
+    <t>ttool</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> desc</t>
+  </si>
+  <si>
+    <t>Experion Whitelabel</t>
+  </si>
+  <si>
+    <t>tool</t>
+  </si>
+  <si>
+    <t>test tool private</t>
+  </si>
+  <si>
+    <t>tool test private</t>
+  </si>
+  <si>
+    <t>private track</t>
+  </si>
+  <si>
+    <t>private add track</t>
+  </si>
+  <si>
+    <t>edit private track</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name </t>
+  </si>
+  <si>
+    <t>track 1</t>
+  </si>
+  <si>
+    <t>test 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> desc1</t>
   </si>
 </sst>
 </file>
@@ -877,10 +916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{455EF352-F706-4455-ADF1-85E3A647B83A}">
-  <dimension ref="A1:P61"/>
+  <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1688,7 +1727,7 @@
         <v>58</v>
       </c>
       <c r="C45" t="s">
-        <v>83</v>
+        <v>148</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -1730,7 +1769,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>130</v>
       </c>
@@ -1741,7 +1780,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>112</v>
       </c>
@@ -1755,7 +1794,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>132</v>
       </c>
@@ -1766,7 +1805,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>115</v>
       </c>
@@ -1783,7 +1822,21 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>148</v>
+      </c>
+      <c r="C53" t="s">
+        <v>144</v>
+      </c>
+      <c r="D53" t="s">
+        <v>146</v>
+      </c>
+      <c r="E53" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
         <v>114</v>
       </c>
@@ -1800,7 +1853,21 @@
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>149</v>
+      </c>
+      <c r="C55" t="s">
+        <v>147</v>
+      </c>
+      <c r="D55" t="s">
+        <v>146</v>
+      </c>
+      <c r="E55" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
         <v>116</v>
       </c>
@@ -1811,15 +1878,15 @@
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>10</v>
       </c>
       <c r="C57" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
         <v>118</v>
       </c>
@@ -1833,7 +1900,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>123</v>
       </c>
@@ -1844,7 +1911,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
         <v>122</v>
       </c>
@@ -1864,7 +1931,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>83</v>
       </c>
@@ -1878,6 +1945,80 @@
         <v>101</v>
       </c>
       <c r="F61" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>151</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>150</v>
+      </c>
+      <c r="C63" t="s">
+        <v>83</v>
+      </c>
+      <c r="D63" t="s">
+        <v>146</v>
+      </c>
+      <c r="E63" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>152</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>154</v>
+      </c>
+      <c r="C65" t="s">
+        <v>155</v>
+      </c>
+      <c r="D65" t="s">
+        <v>146</v>
+      </c>
+      <c r="E65" t="s">
+        <v>156</v>
+      </c>
+      <c r="F65" t="s">
+        <v>101</v>
+      </c>
+      <c r="G65" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>

<commit_message>
assertion added to test cases xml file changed based on methods classes
</commit_message>
<xml_diff>
--- a/salesboost-adminpanel/Excel/Data.xlsx
+++ b/salesboost-adminpanel/Excel/Data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\workspace-spring-tool-suite-4-4.7.0.RELEASE\salesboost-adminpanel\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07804A91-D816-4272-A8F8-E44D85BF7A56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448F5F9C-8D4A-4189-8508-21D1010C2F48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="7" activeTab="11" xr2:uid="{0E4BCD85-B79C-44E4-BF30-FA11BE829E64}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="18000" windowHeight="9360" activeTab="2" xr2:uid="{0E4BCD85-B79C-44E4-BF30-FA11BE829E64}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
-    <sheet name="Manage Passwords" sheetId="2" r:id="rId2"/>
+    <sheet name="ManagePasswords" sheetId="2" r:id="rId2"/>
     <sheet name="UsersData" sheetId="3" r:id="rId3"/>
     <sheet name="AccountHoldersData" sheetId="4" r:id="rId4"/>
     <sheet name="TracksData" sheetId="6" r:id="rId5"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="143">
   <si>
     <t>balu.kr@experionglobal.com</t>
   </si>
@@ -52,21 +52,9 @@
     <t>qI85Jx$3</t>
   </si>
   <si>
-    <t>ayan</t>
-  </si>
-  <si>
     <t>ayan.das+1@experionglobal.com</t>
   </si>
   <si>
-    <t>das</t>
-  </si>
-  <si>
-    <t>Ayan</t>
-  </si>
-  <si>
-    <t>ayan.das+2@experionglobal.com</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -82,30 +70,12 @@
     <t>P</t>
   </si>
   <si>
-    <t>ayan das</t>
-  </si>
-  <si>
-    <t>Ayan sep test</t>
-  </si>
-  <si>
-    <t>ayan.das+7@experionglobal.com</t>
-  </si>
-  <si>
-    <t>Exp</t>
-  </si>
-  <si>
     <t>exp</t>
   </si>
   <si>
-    <t>ayan.das+8@experionglobal.com</t>
-  </si>
-  <si>
     <t>G</t>
   </si>
   <si>
-    <t>Exp Ayan</t>
-  </si>
-  <si>
     <t>login password</t>
   </si>
   <si>
@@ -325,9 +295,6 @@
     <t>Edit Track</t>
   </si>
   <si>
-    <t>test track</t>
-  </si>
-  <si>
     <t>this is  a  test track for aut.</t>
   </si>
   <si>
@@ -388,9 +355,6 @@
     <t>Experion Whitelabel</t>
   </si>
   <si>
-    <t>test tool private</t>
-  </si>
-  <si>
     <t>private track</t>
   </si>
   <si>
@@ -470,6 +434,45 @@
   </si>
   <si>
     <t>Private Edit Tool</t>
+  </si>
+  <si>
+    <t>Exp Automa</t>
+  </si>
+  <si>
+    <t>atmn</t>
+  </si>
+  <si>
+    <t>ayan.das+902@experionglobal.com</t>
+  </si>
+  <si>
+    <t>Automat Exp</t>
+  </si>
+  <si>
+    <t>ayan.das+903@experionglobal.com</t>
+  </si>
+  <si>
+    <t>test auto</t>
+  </si>
+  <si>
+    <t>auto test</t>
+  </si>
+  <si>
+    <t>automate test</t>
+  </si>
+  <si>
+    <t>automate</t>
+  </si>
+  <si>
+    <t>ayan.das+905@experionglobal.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aut. </t>
+  </si>
+  <si>
+    <t>ayan.das+906@experionglobal.com</t>
+  </si>
+  <si>
+    <t>\Image\1.png</t>
   </si>
 </sst>
 </file>
@@ -931,10 +934,10 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -1220,7 +1223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECA8C19-4074-43D4-BE52-F74D129D4AEA}">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1232,137 +1235,137 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B36">
         <v>12</v>
       </c>
       <c r="C36" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="D36" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="E36" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="F36" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="G36" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B64">
         <v>12</v>
       </c>
       <c r="C64" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="D64" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E64" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="F64" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="G64" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="H64" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="I64" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1375,7 +1378,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1398,95 +1401,95 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="8" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="G1" s="9"/>
       <c r="H1" s="8" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="K1" s="9"/>
       <c r="L1" s="7" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="K2" s="9"/>
       <c r="L2" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="E3" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="I3" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="J3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="K3" s="9"/>
       <c r="L3" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="M3" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1643,8 +1646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A17B05B-CFB1-4135-9111-4264EF5F88AF}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1662,85 +1665,85 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="8" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="H1" s="9"/>
       <c r="I1" s="8" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="2" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="G3" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="J3" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="K3" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="L3" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1870,7 +1873,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1881,10 +1884,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1899,8 +1902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEC5848A-912A-4773-8461-544366B3AD23}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1921,84 +1924,84 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="9"/>
       <c r="D1" s="4" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="H1" s="9"/>
       <c r="I1" s="4" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>137</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>139</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>138</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="1" t="s">
-        <v>14</v>
+        <v>141</v>
       </c>
       <c r="J3" t="s">
-        <v>5</v>
+        <v>140</v>
       </c>
       <c r="K3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2123,7 +2126,7 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2146,101 +2149,101 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="J1" s="9"/>
       <c r="K1" s="7" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="J2" s="9"/>
       <c r="K2" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>130</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>130</v>
       </c>
       <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
       <c r="H3" t="s">
-        <v>2</v>
+        <v>131</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>17</v>
+        <v>132</v>
       </c>
       <c r="J3" s="9"/>
       <c r="K3" t="s">
-        <v>12</v>
+        <v>133</v>
       </c>
       <c r="L3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="M3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>6</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -2378,7 +2381,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2396,90 +2399,90 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="8" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="F1" s="11"/>
       <c r="G1" s="9"/>
       <c r="H1" s="8" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="2" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="2" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>135</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" t="s">
+        <v>136</v>
+      </c>
+      <c r="I3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J3" t="s">
+        <v>83</v>
+      </c>
+      <c r="K3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L3" t="s">
         <v>61</v>
-      </c>
-      <c r="I3" t="s">
-        <v>95</v>
-      </c>
-      <c r="J3" t="s">
-        <v>94</v>
-      </c>
-      <c r="K3" t="s">
-        <v>78</v>
-      </c>
-      <c r="L3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2630,101 +2633,101 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="8" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="H1" s="9"/>
       <c r="I1" s="8" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="2" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="G3" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="J3" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="K3" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="L3" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="M3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="N3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -2845,7 +2848,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2864,71 +2867,77 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="7" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="G1" s="9"/>
       <c r="H1" s="7" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>142</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="I3" t="s">
-        <v>111</v>
+        <v>100</v>
+      </c>
+      <c r="J3" t="s">
+        <v>142</v>
       </c>
       <c r="K3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -3066,159 +3075,159 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B35" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C35" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D35" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="E35" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="F35" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="G35" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H35" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G67" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H67" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H67" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="I67" s="2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="J67" s="2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B68" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C68" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D68" t="s">
+        <v>51</v>
+      </c>
+      <c r="E68" t="s">
+        <v>52</v>
+      </c>
+      <c r="F68" t="s">
+        <v>53</v>
+      </c>
+      <c r="G68" t="s">
+        <v>54</v>
+      </c>
+      <c r="H68" t="s">
+        <v>53</v>
+      </c>
+      <c r="I68" t="s">
+        <v>57</v>
+      </c>
+      <c r="J68" t="s">
         <v>61</v>
       </c>
-      <c r="E68" t="s">
-        <v>62</v>
-      </c>
-      <c r="F68" t="s">
-        <v>63</v>
-      </c>
-      <c r="G68" t="s">
-        <v>64</v>
-      </c>
-      <c r="H68" t="s">
-        <v>63</v>
-      </c>
-      <c r="I68" t="s">
-        <v>67</v>
-      </c>
-      <c r="J68" t="s">
-        <v>71</v>
-      </c>
       <c r="K68" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -3230,7 +3239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E86D0F7-BCF6-488F-BA51-24FE603AEB5E}">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="J67" sqref="J67"/>
     </sheetView>
   </sheetViews>
@@ -3244,119 +3253,119 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C33" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D33" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E33" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="F33" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C68" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D68" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="E68" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="F68" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="G68" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
push with changed assertions
</commit_message>
<xml_diff>
--- a/salesboost-adminpanel/Excel/Data.xlsx
+++ b/salesboost-adminpanel/Excel/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\workspace-spring-tool-suite-4-4.7.0.RELEASE\salesboost-adminpanel\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448F5F9C-8D4A-4189-8508-21D1010C2F48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FED662-4A77-4574-865D-B680CCD31163}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="18000" windowHeight="9360" activeTab="2" xr2:uid="{0E4BCD85-B79C-44E4-BF30-FA11BE829E64}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{0E4BCD85-B79C-44E4-BF30-FA11BE829E64}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="148">
   <si>
     <t>balu.kr@experionglobal.com</t>
   </si>
@@ -52,9 +52,6 @@
     <t>qI85Jx$3</t>
   </si>
   <si>
-    <t>ayan.das+1@experionglobal.com</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -70,9 +67,6 @@
     <t>P</t>
   </si>
   <si>
-    <t>exp</t>
-  </si>
-  <si>
     <t>G</t>
   </si>
   <si>
@@ -436,43 +430,64 @@
     <t>Private Edit Tool</t>
   </si>
   <si>
-    <t>Exp Automa</t>
-  </si>
-  <si>
-    <t>atmn</t>
-  </si>
-  <si>
-    <t>ayan.das+902@experionglobal.com</t>
-  </si>
-  <si>
     <t>Automat Exp</t>
   </si>
   <si>
-    <t>ayan.das+903@experionglobal.com</t>
-  </si>
-  <si>
-    <t>test auto</t>
-  </si>
-  <si>
-    <t>auto test</t>
-  </si>
-  <si>
-    <t>automate test</t>
-  </si>
-  <si>
-    <t>automate</t>
-  </si>
-  <si>
-    <t>ayan.das+905@experionglobal.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">Aut. </t>
   </si>
   <si>
-    <t>ayan.das+906@experionglobal.com</t>
-  </si>
-  <si>
     <t>\Image\1.png</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>aytesting0+1@gmail.com</t>
+  </si>
+  <si>
+    <t>autoated</t>
+  </si>
+  <si>
+    <t>test automate</t>
+  </si>
+  <si>
+    <t>automated test</t>
+  </si>
+  <si>
+    <t>automated desc</t>
+  </si>
+  <si>
+    <t>account sel</t>
+  </si>
+  <si>
+    <t>Experion WhiteLabel Training</t>
+  </si>
+  <si>
+    <t>aytesting0+451@gmail.com</t>
+  </si>
+  <si>
+    <t>aytesting0+452@gmail.com</t>
+  </si>
+  <si>
+    <t>automated1</t>
+  </si>
+  <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>Exp1 Automation1</t>
+  </si>
+  <si>
+    <t>aytesting0+455@gmail.com</t>
+  </si>
+  <si>
+    <t>Exp1 Automation scr</t>
+  </si>
+  <si>
+    <t>aytesting0+459@gmail.com</t>
+  </si>
+  <si>
+    <t>ayan test</t>
   </si>
 </sst>
 </file>
@@ -934,10 +949,10 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -1223,7 +1238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECA8C19-4074-43D4-BE52-F74D129D4AEA}">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1235,137 +1250,137 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F35" s="2" t="s">
+      <c r="G35" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B36">
         <v>12</v>
       </c>
       <c r="C36" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D36" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E36" t="s">
+        <v>64</v>
+      </c>
+      <c r="F36" t="s">
         <v>66</v>
       </c>
-      <c r="F36" t="s">
-        <v>68</v>
-      </c>
       <c r="G36" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C63" s="2" t="s">
+      <c r="D63" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="F63" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E63" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F63" s="2" t="s">
+      <c r="G63" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I63" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="G63" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I63" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B64">
         <v>12</v>
       </c>
       <c r="C64" t="s">
+        <v>90</v>
+      </c>
+      <c r="D64" t="s">
+        <v>62</v>
+      </c>
+      <c r="E64" t="s">
+        <v>64</v>
+      </c>
+      <c r="F64" t="s">
         <v>92</v>
       </c>
-      <c r="D64" t="s">
-        <v>64</v>
-      </c>
-      <c r="E64" t="s">
+      <c r="G64" t="s">
         <v>66</v>
       </c>
-      <c r="F64" t="s">
+      <c r="H64" t="s">
+        <v>97</v>
+      </c>
+      <c r="I64" t="s">
         <v>94</v>
-      </c>
-      <c r="G64" t="s">
-        <v>68</v>
-      </c>
-      <c r="H64" t="s">
-        <v>99</v>
-      </c>
-      <c r="I64" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1401,95 +1416,95 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G1" s="9"/>
       <c r="H1" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K1" s="9"/>
       <c r="L1" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K2" s="9"/>
       <c r="L2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K3" s="9"/>
       <c r="L3" t="s">
+        <v>87</v>
+      </c>
+      <c r="M3" t="s">
+        <v>88</v>
+      </c>
+      <c r="N3" s="13" t="s">
         <v>89</v>
-      </c>
-      <c r="M3" t="s">
-        <v>90</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1665,85 +1680,85 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H1" s="9"/>
       <c r="I1" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K3" t="s">
+        <v>100</v>
+      </c>
+      <c r="L3" t="s">
         <v>105</v>
-      </c>
-      <c r="J3" t="s">
-        <v>106</v>
-      </c>
-      <c r="K3" t="s">
-        <v>102</v>
-      </c>
-      <c r="L3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1873,7 +1888,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1884,10 +1899,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1903,7 +1918,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1924,84 +1939,84 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="9"/>
       <c r="D1" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H1" s="9"/>
       <c r="I1" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="1" t="s">
         <v>139</v>
       </c>
       <c r="E3" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
+        <v>142</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J3" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="K3" t="s">
-        <v>8</v>
+        <v>142</v>
       </c>
       <c r="L3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2125,8 +2140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B9674C1-860A-4590-9B39-E42A5F377042}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2149,101 +2164,101 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J1" s="9"/>
       <c r="K1" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="J2" s="9"/>
       <c r="K2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="N2" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>145</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" t="s">
-        <v>5</v>
-      </c>
       <c r="G3" t="s">
-        <v>8</v>
+        <v>133</v>
       </c>
       <c r="H3" t="s">
         <v>131</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="J3" s="9"/>
       <c r="K3" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="L3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -2378,10 +2393,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E7194E-5C36-451D-9FDA-58AB7536DB26}">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2395,145 +2410,152 @@
     <col min="8" max="8" width="10.7109375" customWidth="1"/>
     <col min="10" max="10" width="13.140625" customWidth="1"/>
     <col min="12" max="12" width="16.140625" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F1" s="11"/>
       <c r="G1" s="9"/>
       <c r="H1" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="K2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J3" t="s">
         <v>136</v>
       </c>
-      <c r="I3" t="s">
-        <v>84</v>
-      </c>
-      <c r="J3" t="s">
-        <v>83</v>
-      </c>
       <c r="K3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="M3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C4" s="9"/>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C5" s="9"/>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C7" s="9"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C8" s="9"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C9" s="9"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C10" s="9"/>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C11" s="9"/>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C12" s="9"/>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C13" s="9"/>
       <c r="G13" s="9"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C14" s="9"/>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C15" s="9"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C16" s="9"/>
       <c r="G16" s="9"/>
     </row>
@@ -2612,10 +2634,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21F358C6-80F6-4159-84BF-12DB798ECF6B}">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2629,156 +2651,163 @@
     <col min="11" max="11" width="19.28515625" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
     <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="15" max="15" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H1" s="9"/>
       <c r="I1" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" t="s">
+        <v>103</v>
+      </c>
+      <c r="J3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K3" t="s">
+        <v>100</v>
+      </c>
+      <c r="L3" t="s">
         <v>105</v>
       </c>
-      <c r="J3" t="s">
-        <v>106</v>
-      </c>
-      <c r="K3" t="s">
-        <v>102</v>
-      </c>
-      <c r="L3" t="s">
-        <v>107</v>
-      </c>
       <c r="M3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="N3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="O3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C4" s="9"/>
       <c r="H4" s="9"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C5" s="9"/>
       <c r="H5" s="9"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C6" s="9"/>
       <c r="H6" s="9"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C7" s="9"/>
       <c r="H7" s="9"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C8" s="9"/>
       <c r="H8" s="9"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C9" s="9"/>
       <c r="H9" s="9"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C10" s="9"/>
       <c r="H10" s="9"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C11" s="9"/>
       <c r="H11" s="9"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C12" s="9"/>
       <c r="H12" s="9"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C13" s="9"/>
       <c r="H13" s="9"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C14" s="9"/>
       <c r="H14" s="9"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C15" s="9"/>
       <c r="H15" s="9"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C16" s="9"/>
       <c r="H16" s="9"/>
     </row>
@@ -2867,77 +2896,77 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G1" s="9"/>
       <c r="H1" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="K3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -3057,7 +3086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D621CA-C175-4BB2-BA9E-0B818144D9AC}">
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K68" sqref="K68"/>
     </sheetView>
   </sheetViews>
@@ -3075,159 +3104,159 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="G34" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="H34" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" t="s">
         <v>48</v>
       </c>
-      <c r="B35" t="s">
+      <c r="D35" t="s">
         <v>49</v>
       </c>
-      <c r="C35" t="s">
+      <c r="E35" t="s">
         <v>50</v>
       </c>
-      <c r="D35" t="s">
+      <c r="F35" t="s">
         <v>51</v>
       </c>
-      <c r="E35" t="s">
+      <c r="G35" t="s">
         <v>52</v>
       </c>
-      <c r="F35" t="s">
+      <c r="H35" t="s">
         <v>53</v>
-      </c>
-      <c r="G35" t="s">
-        <v>54</v>
-      </c>
-      <c r="H35" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="D67" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="E67" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="F67" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E67" s="2" t="s">
+      <c r="G67" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F67" s="2" t="s">
+      <c r="H67" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J67" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K67" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I67" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J67" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="K67" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B68" t="s">
+        <v>57</v>
+      </c>
+      <c r="C68" t="s">
+        <v>58</v>
+      </c>
+      <c r="D68" t="s">
+        <v>49</v>
+      </c>
+      <c r="E68" t="s">
+        <v>50</v>
+      </c>
+      <c r="F68" t="s">
+        <v>51</v>
+      </c>
+      <c r="G68" t="s">
+        <v>52</v>
+      </c>
+      <c r="H68" t="s">
+        <v>51</v>
+      </c>
+      <c r="I68" t="s">
+        <v>55</v>
+      </c>
+      <c r="J68" t="s">
         <v>59</v>
       </c>
-      <c r="C68" t="s">
-        <v>60</v>
-      </c>
-      <c r="D68" t="s">
-        <v>51</v>
-      </c>
-      <c r="E68" t="s">
-        <v>52</v>
-      </c>
-      <c r="F68" t="s">
+      <c r="K68" t="s">
         <v>53</v>
-      </c>
-      <c r="G68" t="s">
-        <v>54</v>
-      </c>
-      <c r="H68" t="s">
-        <v>53</v>
-      </c>
-      <c r="I68" t="s">
-        <v>57</v>
-      </c>
-      <c r="J68" t="s">
-        <v>61</v>
-      </c>
-      <c r="K68" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -3239,7 +3268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E86D0F7-BCF6-488F-BA51-24FE603AEB5E}">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="J67" sqref="J67"/>
     </sheetView>
   </sheetViews>
@@ -3253,119 +3282,119 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E32" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" t="s">
         <v>64</v>
       </c>
-      <c r="B33" t="s">
+      <c r="E33" t="s">
         <v>65</v>
       </c>
-      <c r="C33" t="s">
-        <v>51</v>
-      </c>
-      <c r="D33" t="s">
-        <v>66</v>
-      </c>
-      <c r="E33" t="s">
-        <v>67</v>
-      </c>
       <c r="F33" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="C67" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="E67" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D67" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E67" s="2" t="s">
+      <c r="F67" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G67" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B68" t="s">
+        <v>63</v>
+      </c>
+      <c r="C68" t="s">
+        <v>68</v>
+      </c>
+      <c r="D68" t="s">
+        <v>64</v>
+      </c>
+      <c r="E68" t="s">
         <v>65</v>
       </c>
-      <c r="C68" t="s">
-        <v>70</v>
-      </c>
-      <c r="D68" t="s">
-        <v>66</v>
-      </c>
-      <c r="E68" t="s">
-        <v>67</v>
-      </c>
       <c r="F68" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G68" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code with changed assertions for leadership tips and announcements
</commit_message>
<xml_diff>
--- a/salesboost-adminpanel/Excel/Data.xlsx
+++ b/salesboost-adminpanel/Excel/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\workspace-spring-tool-suite-4-4.7.0.RELEASE\salesboost-adminpanel\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FED662-4A77-4574-865D-B680CCD31163}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F495172B-8D56-4216-A79F-45DDA3453030}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{0E4BCD85-B79C-44E4-BF30-FA11BE829E64}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="6" activeTab="7" xr2:uid="{0E4BCD85-B79C-44E4-BF30-FA11BE829E64}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="152">
   <si>
     <t>balu.kr@experionglobal.com</t>
   </si>
@@ -436,9 +436,6 @@
     <t xml:space="preserve">Aut. </t>
   </si>
   <si>
-    <t>\Image\1.png</t>
-  </si>
-  <si>
     <t>user</t>
   </si>
   <si>
@@ -488,6 +485,21 @@
   </si>
   <si>
     <t>ayan test</t>
+  </si>
+  <si>
+    <t>\Images\1.png</t>
+  </si>
+  <si>
+    <t>delete track data</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Delete track</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -518,7 +530,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -573,6 +585,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -587,7 +605,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -606,6 +624,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1238,7 +1257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECA8C19-4074-43D4-BE52-F74D129D4AEA}">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A25" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1902,7 +1921,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1917,7 +1936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEC5848A-912A-4773-8461-544366B3AD23}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1990,30 +2009,30 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F3" t="s">
         <v>141</v>
-      </c>
-      <c r="F3" t="s">
-        <v>142</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J3" t="s">
         <v>129</v>
       </c>
       <c r="K3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L3" t="s">
         <v>2</v>
@@ -2226,11 +2245,11 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -2239,13 +2258,13 @@
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J3" s="9"/>
       <c r="K3" t="s">
@@ -2258,7 +2277,7 @@
         <v>4</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -2393,10 +2412,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E7194E-5C36-451D-9FDA-58AB7536DB26}">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2410,10 +2429,12 @@
     <col min="8" max="8" width="10.7109375" customWidth="1"/>
     <col min="10" max="10" width="13.140625" customWidth="1"/>
     <col min="12" max="12" width="16.140625" customWidth="1"/>
-    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="13" max="13" width="27" customWidth="1"/>
+    <col min="14" max="14" width="0.7109375" customWidth="1"/>
+    <col min="15" max="15" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>74</v>
       </c>
@@ -2432,8 +2453,12 @@
       <c r="I1" s="8" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="14"/>
+      <c r="O1" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -2467,19 +2492,23 @@
         <v>56</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="N2" s="14"/>
+      <c r="O2" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E3" t="s">
         <v>49</v>
@@ -2489,13 +2518,13 @@
       </c>
       <c r="G3" s="9"/>
       <c r="H3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I3" t="s">
         <v>82</v>
       </c>
       <c r="J3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K3" t="s">
         <v>66</v>
@@ -2504,140 +2533,175 @@
         <v>59</v>
       </c>
       <c r="M3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="N3" s="14"/>
+      <c r="O3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C4" s="9"/>
       <c r="G4" s="9"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" s="14"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C5" s="9"/>
       <c r="G5" s="9"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5" s="14"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C6" s="9"/>
       <c r="G6" s="9"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6" s="14"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C7" s="9"/>
       <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" s="14"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C8" s="9"/>
       <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8" s="14"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C9" s="9"/>
       <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9" s="14"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C10" s="9"/>
       <c r="G10" s="9"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10" s="14"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C11" s="9"/>
       <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11" s="14"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C12" s="9"/>
       <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12" s="14"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C13" s="9"/>
       <c r="G13" s="9"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13" s="14"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C14" s="9"/>
       <c r="G14" s="9"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14" s="14"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C15" s="9"/>
       <c r="G15" s="9"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15" s="14"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C16" s="9"/>
       <c r="G16" s="9"/>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="N16" s="14"/>
+    </row>
+    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C17" s="9"/>
       <c r="G17" s="9"/>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="N17" s="14"/>
+    </row>
+    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C18" s="9"/>
       <c r="G18" s="9"/>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="N18" s="14"/>
+    </row>
+    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C19" s="9"/>
       <c r="G19" s="9"/>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="N19" s="14"/>
+    </row>
+    <row r="20" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C20" s="9"/>
       <c r="G20" s="9"/>
-    </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="N20" s="14"/>
+    </row>
+    <row r="21" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C21" s="9"/>
       <c r="G21" s="9"/>
-    </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="N21" s="14"/>
+    </row>
+    <row r="22" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C22" s="9"/>
       <c r="G22" s="9"/>
-    </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="N22" s="14"/>
+    </row>
+    <row r="23" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C23" s="9"/>
       <c r="G23" s="9"/>
-    </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="N23" s="14"/>
+    </row>
+    <row r="24" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C24" s="9"/>
       <c r="G24" s="9"/>
-    </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="N24" s="14"/>
+    </row>
+    <row r="25" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C25" s="9"/>
       <c r="G25" s="9"/>
-    </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="N25" s="14"/>
+    </row>
+    <row r="26" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C26" s="9"/>
       <c r="G26" s="9"/>
-    </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="N26" s="14"/>
+    </row>
+    <row r="27" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C27" s="9"/>
       <c r="G27" s="9"/>
-    </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="N27" s="14"/>
+    </row>
+    <row r="28" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C28" s="9"/>
       <c r="G28" s="9"/>
-    </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="N28" s="14"/>
+    </row>
+    <row r="29" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C29" s="9"/>
       <c r="G29" s="9"/>
-    </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="N29" s="14"/>
+    </row>
+    <row r="30" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C30" s="9"/>
       <c r="G30" s="9"/>
-    </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="N30" s="14"/>
+    </row>
+    <row r="31" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C31" s="9"/>
       <c r="G31" s="9"/>
-    </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="N31" s="14"/>
+    </row>
+    <row r="32" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C32" s="9"/>
       <c r="G32" s="9"/>
-    </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="N32" s="14"/>
+    </row>
+    <row r="33" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C33" s="9"/>
       <c r="G33" s="9"/>
+      <c r="N33" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21F358C6-80F6-4159-84BF-12DB798ECF6B}">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2652,9 +2716,11 @@
     <col min="12" max="12" width="12" customWidth="1"/>
     <col min="14" max="14" width="15.7109375" customWidth="1"/>
     <col min="15" max="15" width="29.140625" customWidth="1"/>
+    <col min="16" max="16" width="1.140625" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>74</v>
       </c>
@@ -2672,8 +2738,12 @@
       <c r="J1" s="8" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" s="14"/>
+      <c r="Q1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -2713,10 +2783,14 @@
         <v>56</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2756,116 +2830,147 @@
         <v>59</v>
       </c>
       <c r="O3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="P3" s="14"/>
+      <c r="Q3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C4" s="9"/>
       <c r="H4" s="9"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4" s="14"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C5" s="9"/>
       <c r="H5" s="9"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5" s="14"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C6" s="9"/>
       <c r="H6" s="9"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6" s="14"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C7" s="9"/>
       <c r="H7" s="9"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7" s="14"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C8" s="9"/>
       <c r="H8" s="9"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8" s="14"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C9" s="9"/>
       <c r="H9" s="9"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9" s="14"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C10" s="9"/>
       <c r="H10" s="9"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P10" s="14"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C11" s="9"/>
       <c r="H11" s="9"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11" s="14"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C12" s="9"/>
       <c r="H12" s="9"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P12" s="14"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C13" s="9"/>
       <c r="H13" s="9"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P13" s="14"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C14" s="9"/>
       <c r="H14" s="9"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P14" s="14"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C15" s="9"/>
       <c r="H15" s="9"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P15" s="14"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C16" s="9"/>
       <c r="H16" s="9"/>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="P16" s="14"/>
+    </row>
+    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C17" s="9"/>
       <c r="H17" s="9"/>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="P17" s="14"/>
+    </row>
+    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C18" s="9"/>
       <c r="H18" s="9"/>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="P18" s="14"/>
+    </row>
+    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C19" s="9"/>
       <c r="H19" s="9"/>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="P19" s="14"/>
+    </row>
+    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C20" s="9"/>
       <c r="H20" s="9"/>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="P20" s="14"/>
+    </row>
+    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C21" s="9"/>
       <c r="H21" s="9"/>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="P21" s="14"/>
+    </row>
+    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C22" s="9"/>
       <c r="H22" s="9"/>
-    </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="P22" s="14"/>
+    </row>
+    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C23" s="9"/>
       <c r="H23" s="9"/>
-    </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="P23" s="14"/>
+    </row>
+    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C24" s="9"/>
       <c r="H24" s="9"/>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="P24" s="14"/>
+    </row>
+    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C25" s="9"/>
       <c r="H25" s="9"/>
-    </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="P25" s="14"/>
+    </row>
+    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C26" s="9"/>
       <c r="H26" s="9"/>
-    </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="P26" s="14"/>
+    </row>
+    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C27" s="9"/>
       <c r="H27" s="9"/>
-    </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="P27" s="14"/>
+    </row>
+    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C28" s="9"/>
       <c r="H28" s="9"/>
-    </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="P28" s="14"/>
+    </row>
+    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C29" s="9"/>
       <c r="H29" s="9"/>
-    </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="P29" s="14"/>
+    </row>
+    <row r="30" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C30" s="9"/>
       <c r="H30" s="9"/>
+      <c r="P30" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2953,7 +3058,7 @@
         <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" t="s">
@@ -2963,7 +3068,7 @@
         <v>98</v>
       </c>
       <c r="J3" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="K3" t="s">
         <v>2</v>
@@ -3086,8 +3191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D621CA-C175-4BB2-BA9E-0B818144D9AC}">
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K68" sqref="K68"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Smoke Suite Code in whole along with OR's and test scripts
</commit_message>
<xml_diff>
--- a/salesboost-adminpanel/Excel/Data.xlsx
+++ b/salesboost-adminpanel/Excel/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\workspace-spring-tool-suite-4-4.7.0.RELEASE\salesboost-adminpanel\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SB\salesboost-adminpanel(New)\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F495172B-8D56-4216-A79F-45DDA3453030}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1387AB-5B4D-45B9-8ED6-9AAE84CB2EB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="6" activeTab="7" xr2:uid="{0E4BCD85-B79C-44E4-BF30-FA11BE829E64}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
@@ -25,26 +25,25 @@
     <sheet name="LeadershipTipData" sheetId="11" r:id="rId10"/>
     <sheet name="LeadershipToolData" sheetId="12" r:id="rId11"/>
     <sheet name="PrivateLeadershipToolData" sheetId="13" r:id="rId12"/>
+    <sheet name="AddCourse" sheetId="14" r:id="rId13"/>
+    <sheet name="LAT" sheetId="15" r:id="rId14"/>
+    <sheet name="PVO" sheetId="16" r:id="rId15"/>
+    <sheet name="FAQ" sheetId="17" r:id="rId16"/>
+    <sheet name="ATA" sheetId="18" r:id="rId17"/>
+    <sheet name="AssociatedFiles" sheetId="19" r:id="rId18"/>
+    <sheet name="Awards" sheetId="20" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="230">
   <si>
     <t>balu.kr@experionglobal.com</t>
   </si>
@@ -136,18 +135,12 @@
     <t>description</t>
   </si>
   <si>
-    <t>test role</t>
-  </si>
-  <si>
     <t>test description</t>
   </si>
   <si>
     <t>role list</t>
   </si>
   <si>
-    <t>role test</t>
-  </si>
-  <si>
     <t>System announcements</t>
   </si>
   <si>
@@ -184,15 +177,6 @@
     <t>content</t>
   </si>
   <si>
-    <t>test announcement</t>
-  </si>
-  <si>
-    <t>test acc</t>
-  </si>
-  <si>
-    <t>abc</t>
-  </si>
-  <si>
     <t>test</t>
   </si>
   <si>
@@ -217,9 +201,6 @@
     <t>courses</t>
   </si>
   <si>
-    <t>test accts</t>
-  </si>
-  <si>
     <t>abc.com</t>
   </si>
   <si>
@@ -235,9 +216,6 @@
     <t>test tip</t>
   </si>
   <si>
-    <t>testtip</t>
-  </si>
-  <si>
     <t>desc</t>
   </si>
   <si>
@@ -247,9 +225,6 @@
     <t>ttc</t>
   </si>
   <si>
-    <t>test tips</t>
-  </si>
-  <si>
     <t>tes tip</t>
   </si>
   <si>
@@ -295,21 +270,12 @@
     <t>track test</t>
   </si>
   <si>
-    <t>test tool</t>
-  </si>
-  <si>
     <t>tts</t>
   </si>
   <si>
-    <t>tool test</t>
-  </si>
-  <si>
     <t>ttt</t>
   </si>
   <si>
-    <t>duplicate test tool</t>
-  </si>
-  <si>
     <t>dtt</t>
   </si>
   <si>
@@ -319,9 +285,6 @@
     <t>test slug</t>
   </si>
   <si>
-    <t>tip test</t>
-  </si>
-  <si>
     <t>tc</t>
   </si>
   <si>
@@ -349,15 +312,9 @@
     <t>Experion Whitelabel</t>
   </si>
   <si>
-    <t>private track</t>
-  </si>
-  <si>
     <t xml:space="preserve">name </t>
   </si>
   <si>
-    <t>track 1</t>
-  </si>
-  <si>
     <t>test 1</t>
   </si>
   <si>
@@ -430,27 +387,12 @@
     <t>Private Edit Tool</t>
   </si>
   <si>
-    <t>Automat Exp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aut. </t>
-  </si>
-  <si>
     <t>user</t>
   </si>
   <si>
-    <t>aytesting0+1@gmail.com</t>
-  </si>
-  <si>
     <t>autoated</t>
   </si>
   <si>
-    <t>test automate</t>
-  </si>
-  <si>
-    <t>automated test</t>
-  </si>
-  <si>
     <t>automated desc</t>
   </si>
   <si>
@@ -460,33 +402,6 @@
     <t>Experion WhiteLabel Training</t>
   </si>
   <si>
-    <t>aytesting0+451@gmail.com</t>
-  </si>
-  <si>
-    <t>aytesting0+452@gmail.com</t>
-  </si>
-  <si>
-    <t>automated1</t>
-  </si>
-  <si>
-    <t>user1</t>
-  </si>
-  <si>
-    <t>Exp1 Automation1</t>
-  </si>
-  <si>
-    <t>aytesting0+455@gmail.com</t>
-  </si>
-  <si>
-    <t>Exp1 Automation scr</t>
-  </si>
-  <si>
-    <t>aytesting0+459@gmail.com</t>
-  </si>
-  <si>
-    <t>ayan test</t>
-  </si>
-  <si>
     <t>\Images\1.png</t>
   </si>
   <si>
@@ -500,13 +415,331 @@
   </si>
   <si>
     <t>E</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Course Name</t>
+  </si>
+  <si>
+    <t>Course short name</t>
+  </si>
+  <si>
+    <t>Course slug</t>
+  </si>
+  <si>
+    <t>Course Privacy</t>
+  </si>
+  <si>
+    <t>Course version status</t>
+  </si>
+  <si>
+    <t>Course description</t>
+  </si>
+  <si>
+    <t>Course video preview URL</t>
+  </si>
+  <si>
+    <t>Certified course checkbox</t>
+  </si>
+  <si>
+    <t>FILTER LIST</t>
+  </si>
+  <si>
+    <t>TestCourseSript</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>Test Course created via script</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>inactive</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>LAT</t>
+  </si>
+  <si>
+    <t>Video Url</t>
+  </si>
+  <si>
+    <t>Video name</t>
+  </si>
+  <si>
+    <t>Video description</t>
+  </si>
+  <si>
+    <t>Test Video 1</t>
+  </si>
+  <si>
+    <t>Test video 12 description</t>
+  </si>
+  <si>
+    <t>PVO</t>
+  </si>
+  <si>
+    <t>Poster Url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Video name </t>
+  </si>
+  <si>
+    <t>Score Based</t>
+  </si>
+  <si>
+    <t>Minimum pass mark</t>
+  </si>
+  <si>
+    <t>Equal weightage</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Wrong answer</t>
+  </si>
+  <si>
+    <t>Correct checkbox</t>
+  </si>
+  <si>
+    <t>Correct answer</t>
+  </si>
+  <si>
+    <t>Test video1</t>
+  </si>
+  <si>
+    <t>Test video 1 description</t>
+  </si>
+  <si>
+    <t>Is this a test?</t>
+  </si>
+  <si>
+    <t>No it is not</t>
+  </si>
+  <si>
+    <t>Yes it is a test</t>
+  </si>
+  <si>
+    <t>FAQ</t>
+  </si>
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Answers</t>
+  </si>
+  <si>
+    <t>Yes, it is</t>
+  </si>
+  <si>
+    <t>ATA</t>
+  </si>
+  <si>
+    <t>Intro text</t>
+  </si>
+  <si>
+    <t>Audio snippet</t>
+  </si>
+  <si>
+    <t>Ideal Test ID</t>
+  </si>
+  <si>
+    <t>Test snippet URL</t>
+  </si>
+  <si>
+    <t>Snippet Description</t>
+  </si>
+  <si>
+    <t>When the call connects, please listen carefully to the audio instructions!</t>
+  </si>
+  <si>
+    <t>Test snippet</t>
+  </si>
+  <si>
+    <t>Associated files</t>
+  </si>
+  <si>
+    <t>File Url</t>
+  </si>
+  <si>
+    <t>Link Text</t>
+  </si>
+  <si>
+    <t>File test 2</t>
+  </si>
+  <si>
+    <t>Award</t>
+  </si>
+  <si>
+    <t>Signatory drop down</t>
+  </si>
+  <si>
+    <t>Sign name</t>
+  </si>
+  <si>
+    <t>Sign title</t>
+  </si>
+  <si>
+    <t>Sign png upload</t>
+  </si>
+  <si>
+    <t>Logo png upload</t>
+  </si>
+  <si>
+    <t>Testing Site</t>
+  </si>
+  <si>
+    <t>Test Name</t>
+  </si>
+  <si>
+    <t>Test Title1</t>
+  </si>
+  <si>
+    <t>ashwin.harikrishnan@experionglobal.com</t>
+  </si>
+  <si>
+    <t>test role 2</t>
+  </si>
+  <si>
+    <t>role test 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Edit snippet</t>
+  </si>
+  <si>
+    <t>Edit snippet test</t>
+  </si>
+  <si>
+    <t>Edit Link Text</t>
+  </si>
+  <si>
+    <t>Edit file test 3</t>
+  </si>
+  <si>
+    <t>\Resources\Imaages\text2.png</t>
+  </si>
+  <si>
+    <t>\Resources\Video\TEST VIDEO.mp4</t>
+  </si>
+  <si>
+    <t>\Resources\Audio\intro.wav</t>
+  </si>
+  <si>
+    <t>Search parameters</t>
+  </si>
+  <si>
+    <t>Course Four</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>private track test 1</t>
+  </si>
+  <si>
+    <t>track test 1</t>
+  </si>
+  <si>
+    <t>test announcement 2</t>
+  </si>
+  <si>
+    <t>test tips edit 1</t>
+  </si>
+  <si>
+    <t>testtipedit</t>
+  </si>
+  <si>
+    <t>tip test edit 2</t>
+  </si>
+  <si>
+    <t>test tool test 1</t>
+  </si>
+  <si>
+    <t>tool test edit 1</t>
+  </si>
+  <si>
+    <t>duplicate test tool 1</t>
+  </si>
+  <si>
+    <t>track 1 test 1</t>
+  </si>
+  <si>
+    <t>Test-Track3</t>
+  </si>
+  <si>
+    <t>Test-Track4</t>
+  </si>
+  <si>
+    <t>abc2</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>test announcement 3</t>
+  </si>
+  <si>
+    <t>test tip 2</t>
+  </si>
+  <si>
+    <t>testtip 2</t>
+  </si>
+  <si>
+    <t>test 2</t>
+  </si>
+  <si>
+    <t>test tip 1</t>
+  </si>
+  <si>
+    <t>Aut User</t>
+  </si>
+  <si>
+    <t>User Aut</t>
+  </si>
+  <si>
+    <t>Aut User B</t>
+  </si>
+  <si>
+    <t>autuserA@yopmail.com</t>
+  </si>
+  <si>
+    <t>autuser2@yopmail.com</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>Auto User A</t>
+  </si>
+  <si>
+    <t>autuseraccnt@yopmail.com</t>
+  </si>
+  <si>
+    <t>edited account</t>
+  </si>
+  <si>
+    <t>uatuseracc@yopmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -529,8 +762,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -591,6 +832,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -605,7 +852,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -625,6 +872,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -939,7 +1190,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{455EF352-F706-4455-ADF1-85E3A647B83A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1254,10 +1505,12 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECA8C19-4074-43D4-BE52-F74D129D4AEA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1269,15 +1522,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1285,121 +1538,121 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>219</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F35" s="2" t="s">
+      <c r="G35" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>219</v>
       </c>
       <c r="B36">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C36" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D36" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E36" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F36" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="G36" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C63" s="2" t="s">
+      <c r="D63" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="F63" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E63" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F63" s="2" t="s">
+      <c r="G63" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I63" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="G63" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I63" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>91</v>
+        <v>206</v>
       </c>
       <c r="B64">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C64" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D64" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E64" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F64" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G64" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="H64" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="I64" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1408,11 +1661,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78607A9B-B63C-4C9C-B954-1F7C84427419}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1435,19 +1688,19 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="8" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="G1" s="9"/>
       <c r="H1" s="8" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="K1" s="9"/>
       <c r="L1" s="7" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1455,14 +1708,14 @@
         <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>29</v>
@@ -1472,7 +1725,7 @@
         <v>28</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>29</v>
@@ -1482,48 +1735,48 @@
         <v>28</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>207</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" t="s">
-        <v>83</v>
+        <v>207</v>
       </c>
       <c r="E3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F3" t="s">
         <v>29</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" t="s">
-        <v>85</v>
+        <v>208</v>
       </c>
       <c r="I3" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="J3" t="s">
         <v>29</v>
       </c>
       <c r="K3" s="9"/>
       <c r="L3" t="s">
-        <v>87</v>
+        <v>209</v>
       </c>
       <c r="M3" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1677,11 +1930,11 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A17B05B-CFB1-4135-9111-4264EF5F88AF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1699,15 +1952,15 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="8" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="H1" s="9"/>
       <c r="I1" s="8" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1715,33 +1968,33 @@
         <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="2" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
@@ -1751,33 +2004,33 @@
         <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>201</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" t="s">
-        <v>101</v>
+        <v>201</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F3" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="G3" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" t="s">
-        <v>103</v>
+        <v>210</v>
       </c>
       <c r="J3" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="K3" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="L3" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1902,12 +2155,597 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:O8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="N1" s="15"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="H2" t="s">
+        <v>138</v>
+      </c>
+      <c r="I2" t="s">
+        <v>196</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="M2" t="s">
+        <v>139</v>
+      </c>
+      <c r="N2" t="s">
+        <v>140</v>
+      </c>
+      <c r="O2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <v>9</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3">
+        <v>11</v>
+      </c>
+      <c r="M3">
+        <v>12</v>
+      </c>
+      <c r="N3">
+        <v>113</v>
+      </c>
+      <c r="O3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="B7" s="15"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="15"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="B7" s="15"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="F3">
+        <v>35</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="H3" t="s">
+        <v>160</v>
+      </c>
+      <c r="I3" t="s">
+        <v>161</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="K3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4">
+        <v>7</v>
+      </c>
+      <c r="I4">
+        <v>8</v>
+      </c>
+      <c r="J4">
+        <v>9</v>
+      </c>
+      <c r="K4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="B7" s="15"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="B7" s="15"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="B7" s="15"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="B7" s="15"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="B7" s="15"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{900EA0C5-B10D-4ACE-B011-B42DAC8CA455}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1921,23 +2759,23 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>131</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{957A2A9B-D581-4055-BB37-2A04B7989113}"/>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEC5848A-912A-4773-8461-544366B3AD23}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1958,16 +2796,16 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="9"/>
       <c r="D1" s="4" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="H1" s="9"/>
       <c r="I1" s="4" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2009,30 +2847,30 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>222</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E3" t="s">
-        <v>140</v>
+        <v>223</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>220</v>
       </c>
       <c r="F3" t="s">
-        <v>141</v>
+        <v>3</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="1" t="s">
-        <v>139</v>
+        <v>224</v>
       </c>
       <c r="J3" t="s">
-        <v>129</v>
+        <v>221</v>
       </c>
       <c r="K3" t="s">
-        <v>141</v>
+        <v>225</v>
       </c>
       <c r="L3" t="s">
         <v>2</v>
@@ -2148,18 +2986,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{D0AFE3BE-50BB-47E1-A32C-109A4C34413E}"/>
-    <hyperlink ref="I3" r:id="rId2" xr:uid="{7EB3832F-C0D7-4D6C-A39D-F40B1E8FC999}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B9674C1-860A-4590-9B39-E42A5F377042}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
@@ -2183,21 +3021,21 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="J1" s="9"/>
       <c r="K1" s="7" t="s">
         <v>25</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -2245,11 +3083,11 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
+        <v>226</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" t="s">
-        <v>142</v>
+        <v>226</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -2258,17 +3096,17 @@
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="H3" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>143</v>
+        <v>227</v>
       </c>
       <c r="J3" s="9"/>
       <c r="K3" t="s">
-        <v>128</v>
+        <v>228</v>
       </c>
       <c r="L3" t="s">
         <v>6</v>
@@ -2277,7 +3115,7 @@
         <v>4</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>145</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -2402,8 +3240,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I3" r:id="rId1" xr:uid="{3527648E-090B-4D92-9615-487DE55EA7EC}"/>
-    <hyperlink ref="N3" r:id="rId2" xr:uid="{9B18CED8-52FE-4C59-8AF8-212812836215}"/>
+    <hyperlink ref="I3" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="N3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -2411,11 +3249,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E7194E-5C36-451D-9FDA-58AB7536DB26}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2436,67 +3274,67 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="8" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="F1" s="11"/>
       <c r="G1" s="9"/>
       <c r="H1" s="8" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="N1" s="14"/>
       <c r="O1" s="8" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="N2" s="14"/>
       <c r="O2" s="2" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -2504,40 +3342,40 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>133</v>
+        <v>211</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" t="s">
-        <v>133</v>
+        <v>211</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" t="s">
-        <v>134</v>
+        <v>212</v>
       </c>
       <c r="I3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="J3" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="K3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="L3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="M3" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="N3" s="14"/>
       <c r="O3" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -2697,11 +3535,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21F358C6-80F6-4159-84BF-12DB798ECF6B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2722,72 +3560,72 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="8" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="H1" s="9"/>
       <c r="I1" s="8" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="P1" s="14"/>
       <c r="Q1" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="2" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="P2" s="14"/>
       <c r="Q2" s="2" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -2795,46 +3633,46 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>201</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" t="s">
-        <v>101</v>
+        <v>201</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F3" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="G3" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" t="s">
-        <v>103</v>
+        <v>202</v>
       </c>
       <c r="J3" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="K3" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="L3" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="M3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="N3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="O3" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="P3" s="14"/>
       <c r="Q3" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -2978,11 +3816,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16C790B7-212B-4535-92F6-ED7DC1A63620}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3001,15 +3839,15 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="7" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="G1" s="9"/>
       <c r="H1" s="7" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -3017,7 +3855,7 @@
         <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="2" t="s">
@@ -3027,7 +3865,7 @@
         <v>29</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="2" t="s">
@@ -3037,10 +3875,10 @@
         <v>29</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -3048,27 +3886,27 @@
         <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>189</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E3" t="s">
         <v>30</v>
       </c>
-      <c r="E3" t="s">
-        <v>31</v>
-      </c>
       <c r="F3" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" t="s">
-        <v>33</v>
+        <v>190</v>
       </c>
       <c r="I3" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="J3" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="K3" t="s">
         <v>2</v>
@@ -3188,11 +4026,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D621CA-C175-4BB2-BA9E-0B818144D9AC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3209,19 +4047,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3229,139 +4067,139 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>203</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="G34" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="H34" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>203</v>
+      </c>
+      <c r="B35" t="s">
+        <v>203</v>
+      </c>
+      <c r="C35" t="s">
+        <v>213</v>
+      </c>
+      <c r="D35" t="s">
+        <v>214</v>
+      </c>
+      <c r="E35" t="s">
+        <v>45</v>
+      </c>
+      <c r="F35" t="s">
         <v>46</v>
       </c>
-      <c r="B35" t="s">
+      <c r="G35" t="s">
         <v>47</v>
       </c>
-      <c r="C35" t="s">
+      <c r="H35" t="s">
         <v>48</v>
-      </c>
-      <c r="D35" t="s">
-        <v>49</v>
-      </c>
-      <c r="E35" t="s">
-        <v>50</v>
-      </c>
-      <c r="F35" t="s">
-        <v>51</v>
-      </c>
-      <c r="G35" t="s">
-        <v>52</v>
-      </c>
-      <c r="H35" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="D67" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="E67" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="F67" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E67" s="2" t="s">
+      <c r="G67" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F67" s="2" t="s">
+      <c r="H67" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J67" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K67" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I67" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J67" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="K67" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>215</v>
+      </c>
+      <c r="B68" t="s">
+        <v>215</v>
+      </c>
+      <c r="C68" t="s">
+        <v>52</v>
+      </c>
+      <c r="D68" t="s">
+        <v>44</v>
+      </c>
+      <c r="E68" t="s">
+        <v>45</v>
+      </c>
+      <c r="F68" t="s">
         <v>46</v>
       </c>
-      <c r="B68" t="s">
-        <v>57</v>
-      </c>
-      <c r="C68" t="s">
-        <v>58</v>
-      </c>
-      <c r="D68" t="s">
-        <v>49</v>
-      </c>
-      <c r="E68" t="s">
+      <c r="G68" t="s">
+        <v>47</v>
+      </c>
+      <c r="H68" t="s">
+        <v>46</v>
+      </c>
+      <c r="I68" t="s">
         <v>50</v>
       </c>
-      <c r="F68" t="s">
-        <v>51</v>
-      </c>
-      <c r="G68" t="s">
-        <v>52</v>
-      </c>
-      <c r="H68" t="s">
-        <v>51</v>
-      </c>
-      <c r="I68" t="s">
-        <v>55</v>
-      </c>
       <c r="J68" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="K68" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -3370,11 +4208,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E86D0F7-BCF6-488F-BA51-24FE603AEB5E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="J67" sqref="J67"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3387,15 +4225,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3403,103 +4241,103 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>216</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E32" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>216</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>217</v>
       </c>
       <c r="C33" t="s">
-        <v>49</v>
+        <v>218</v>
       </c>
       <c r="D33" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E33" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="F33" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="C67" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="E67" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D67" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E67" s="2" t="s">
+      <c r="F67" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G67" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>67</v>
+        <v>204</v>
       </c>
       <c r="B68" t="s">
-        <v>63</v>
+        <v>205</v>
       </c>
       <c r="C68" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D68" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E68" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="F68" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="G68" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
regression script for administrators,account holders,managepass,leadershiptools
</commit_message>
<xml_diff>
--- a/salesboost-adminpanel/Excel/Data.xlsx
+++ b/salesboost-adminpanel/Excel/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SB\salesboost-adminpanel(New)\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1387AB-5B4D-45B9-8ED6-9AAE84CB2EB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF3EAEA-22CA-4ADD-AFBF-14885B6E61A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
@@ -771,7 +771,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -838,6 +838,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -852,7 +858,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -876,6 +882,7 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2772,10 +2779,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2792,9 +2799,12 @@
     <col min="10" max="10" width="16.28515625" customWidth="1"/>
     <col min="11" max="11" width="15.7109375" customWidth="1"/>
     <col min="12" max="12" width="30.5703125" customWidth="1"/>
+    <col min="13" max="13" width="0.42578125" customWidth="1"/>
+    <col min="14" max="14" width="12" customWidth="1"/>
+    <col min="15" max="15" width="0.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>94</v>
       </c>
@@ -2807,8 +2817,11 @@
       <c r="I1" s="4" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="19"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="5"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -2841,8 +2854,11 @@
       <c r="L2" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="19"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2875,114 +2891,170 @@
       <c r="L3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="19"/>
+      <c r="O3" s="5"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C4" s="9"/>
       <c r="H4" s="9"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="19"/>
+      <c r="O4" s="5"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C5" s="9"/>
       <c r="H5" s="9"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" s="19"/>
+      <c r="O5" s="5"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C6" s="9"/>
       <c r="H6" s="9"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" s="19"/>
+      <c r="O6" s="5"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C7" s="9"/>
       <c r="H7" s="9"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" s="19"/>
+      <c r="O7" s="5"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C8" s="9"/>
       <c r="H8" s="9"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" s="19"/>
+      <c r="O8" s="5"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C9" s="9"/>
       <c r="H9" s="9"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" s="19"/>
+      <c r="O9" s="5"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C10" s="9"/>
       <c r="H10" s="9"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" s="19"/>
+      <c r="O10" s="5"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C11" s="9"/>
       <c r="H11" s="9"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" s="19"/>
+      <c r="O11" s="5"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C12" s="9"/>
       <c r="H12" s="9"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" s="19"/>
+      <c r="O12" s="5"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C13" s="9"/>
       <c r="H13" s="9"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" s="19"/>
+      <c r="O13" s="5"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C14" s="9"/>
       <c r="H14" s="9"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" s="19"/>
+      <c r="O14" s="5"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C15" s="9"/>
       <c r="H15" s="9"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" s="19"/>
+      <c r="O15" s="5"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C16" s="9"/>
       <c r="H16" s="9"/>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="M16" s="19"/>
+      <c r="O16" s="5"/>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C17" s="9"/>
       <c r="H17" s="9"/>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="M17" s="19"/>
+      <c r="O17" s="5"/>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C18" s="9"/>
       <c r="H18" s="9"/>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="M18" s="19"/>
+      <c r="O18" s="5"/>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C19" s="9"/>
       <c r="H19" s="9"/>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="M19" s="19"/>
+      <c r="O19" s="5"/>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C20" s="9"/>
       <c r="H20" s="9"/>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="M20" s="19"/>
+      <c r="O20" s="5"/>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C21" s="9"/>
       <c r="H21" s="9"/>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="M21" s="19"/>
+      <c r="O21" s="5"/>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C22" s="9"/>
       <c r="H22" s="9"/>
-    </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="M22" s="19"/>
+      <c r="O22" s="5"/>
+    </row>
+    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C23" s="9"/>
       <c r="H23" s="9"/>
-    </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="M23" s="19"/>
+      <c r="O23" s="5"/>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C24" s="9"/>
       <c r="H24" s="9"/>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="M24" s="19"/>
+      <c r="O24" s="5"/>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C25" s="9"/>
       <c r="H25" s="9"/>
-    </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="M25" s="19"/>
+      <c r="O25" s="5"/>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C26" s="9"/>
       <c r="H26" s="9"/>
-    </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="M26" s="19"/>
+      <c r="O26" s="5"/>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C27" s="9"/>
       <c r="H27" s="9"/>
-    </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="M27" s="19"/>
+      <c r="O27" s="5"/>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C28" s="9"/>
       <c r="H28" s="9"/>
-    </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="M28" s="19"/>
+      <c r="O28" s="5"/>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C29" s="9"/>
       <c r="H29" s="9"/>
-    </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="M29" s="19"/>
+      <c r="O29" s="5"/>
+    </row>
+    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C30" s="9"/>
       <c r="H30" s="9"/>
+      <c r="M30" s="19"/>
+      <c r="O30" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2990,6 +3062,7 @@
     <hyperlink ref="I3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2997,7 +3070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>

</xml_diff>